<commit_message>
Refactored script for better maintainability and execution (Azure SQL to MS SQL rename, DataFrame name changes)
This commit refactors the Python script (ms_sql_to_excel.py) for improved clarity and functionality. Here are the key changes:
 * Renamed references to Azure SQL: Replaced occurrences of "Azure SQL" with "MS SQL" to reflect the actual database type.
 * Updated script execution: Modified the script call in the README to include the required date argument (YYYY-MM-DD) for better execution clarity.
 * DataFrame name changes:
  * Renamed DataFrame keys from "Journals to Expenses" to "Journals to expenses" (lowercase "e") for consistency.
  * Introduced invoice date formatting for DataFrame names in both "Journals to expenses" and "Sales Receipts" for easier identification in the Excel report.
These changes enhance readability, maintainability, and proper execution of the script.
</commit_message>
<xml_diff>
--- a/INVOICE REPORT.xlsx
+++ b/INVOICE REPORT.xlsx
@@ -7,8 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sales_Receipts" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="20211021-Journals to Expenses" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="20231021-Journals to expenses" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sales Receipts-Oct21" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,184 +437,494 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Sales Receipt No</t>
+          <t>Ref No</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Customer</t>
+          <t>Payment Date</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Sales Receipt Date</t>
+          <t>Memo</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Deposit To</t>
+          <t>Account</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Payment method</t>
+          <t>Expense Account</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Global Tax Calculation</t>
+          <t>Expense Line Amount</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Product/Service</t>
+          <t>Expense Description</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Product/Service Description</t>
+          <t>Payee</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Product/Service Amount</t>
+          <t>Expense Class</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Product/Service Class</t>
+          <t>Payment Method</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2021/1021</t>
+          <t>046286</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Cash Sales</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>21/10/2021</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>10300</v>
-      </c>
-      <c r="E2" t="inlineStr">
+          <t>21/10/2023</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="n">
+        <v>52300</v>
+      </c>
+      <c r="F2" t="n">
+        <v>2500</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>TRANSPORTATION</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Petty Cash</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>JUICI</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
         <is>
           <t>Cash</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>NotApplicable</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Cash Sales - Other</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="n">
-        <v>281034.29</v>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>JUICI</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2021/1021</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr"/>
+          <t>046285</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>21/10/2023</t>
+        </is>
+      </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>NotApplicable</t>
-        </is>
+      <c r="E3" t="n">
+        <v>52300</v>
+      </c>
+      <c r="F3" t="n">
+        <v>2500</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Cash Sales - Beverages</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="n">
-        <v>329726.12</v>
+          <t>TRANSPORTATION</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Petty Cash</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>JUICI</t>
+        </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>JUICI</t>
+          <t>Cash</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2021/1021</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr"/>
+          <t>046336</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>21/10/2023</t>
+        </is>
+      </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>NotApplicable</t>
-        </is>
+      <c r="E4" t="n">
+        <v>52300</v>
+      </c>
+      <c r="F4" t="n">
+        <v>2500</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Cash Sales - Juici</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="n">
-        <v>2973946.11</v>
+          <t>TRANSPORTATION</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Petty Cash</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>JUICI</t>
+        </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>JUICI</t>
+          <t>Cash</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2021/1021</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr"/>
+          <t>1944</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>21/10/2023</t>
+        </is>
+      </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>NotApplicable</t>
-        </is>
+      <c r="E5" t="n">
+        <v>52300</v>
+      </c>
+      <c r="F5" t="n">
+        <v>2500</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>12260 GCT Payable/Receivable</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="n">
-        <v>488246.387</v>
-      </c>
-      <c r="J5" t="inlineStr"/>
+          <t>TRANSPORTATION</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Petty Cash</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>JUICI</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>1958</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>21/10/2023</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="n">
+        <v>52300</v>
+      </c>
+      <c r="F6" t="n">
+        <v>2500</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>TRANSPORTATION</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Petty Cash</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>JUICI</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>15637252</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>21/10/2023</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="n">
+        <v>51300</v>
+      </c>
+      <c r="F7" t="n">
+        <v>125</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>TELEPHONE</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Petty Cash</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>JUICI</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>52031232</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>21/10/2023</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="n">
+        <v>51300</v>
+      </c>
+      <c r="F8" t="n">
+        <v>150</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>TELEPHONE</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Petty Cash</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>JUICI</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>797202</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>21/10/2023</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="n">
+        <v>61940</v>
+      </c>
+      <c r="F9" t="n">
+        <v>50</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>ADMINISTRATION</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Petty Cash</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>JUICI</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>G0579929</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>21/10/2023</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="n">
+        <v>67200</v>
+      </c>
+      <c r="F10" t="n">
+        <v>2500.01</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>REPAIR&amp;MAIN</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Petty Cash</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>JUICI</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>JFB-DON-191023</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>21/10/2023</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="n">
+        <v>61950</v>
+      </c>
+      <c r="F11" t="n">
+        <v>15000</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>MISCELLANEOUS</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Petty Cash</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>JUICI</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>046359</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>21/10/2023</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="n">
+        <v>52300</v>
+      </c>
+      <c r="F12" t="n">
+        <v>2500</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>TRANSPORTATION</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Petty Cash</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>JUICI</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -627,7 +937,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -638,54 +948,184 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Ref No</t>
+          <t>Sales Receipt No</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Payment Date</t>
+          <t>Customer</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Memo</t>
+          <t>Sales Receipt Date</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Account</t>
+          <t>Deposit To</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Expense Account</t>
+          <t>Payment method</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Expense Line Amount</t>
+          <t>Global Tax Calculation</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Expense Description</t>
+          <t>Product/Service</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Payee</t>
+          <t>Product/Service Description</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Expense Class</t>
+          <t>Product/Service Amount</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Payment Method</t>
-        </is>
-      </c>
+          <t>Product/Service Class</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2023/1021</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Cash Sales</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>21/10/2023</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>10300</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>NotApplicable</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Cash Sales - Other</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="n">
+        <v>569497.87</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>JUICI</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2023/1021</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>NotApplicable</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Cash Sales - Beverages</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="n">
+        <v>523085.8</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>JUICI</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2023/1021</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>NotApplicable</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Cash Sales - Juici</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="n">
+        <v>5245213.22</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>JUICI</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2023/1021</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>NotApplicable</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>12260 GCT Payable/Receivable</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="n">
+        <v>872204.4300000001</v>
+      </c>
+      <c r="J5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>